<commit_message>
update frontend (add schedule scheme: add rules)
</commit_message>
<xml_diff>
--- a/ttf-backend/src/main/resources/db/scheme.xls.xlsx
+++ b/ttf-backend/src/main/resources/db/scheme.xls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
   <si>
     <t>Id</t>
   </si>
@@ -90,12 +90,6 @@
   </si>
   <si>
     <t>game_total_player2</t>
-  </si>
-  <si>
-    <t>score_set_total_player1</t>
-  </si>
-  <si>
-    <t>score_set_total_player2</t>
   </si>
   <si>
     <t>score_set1_player1</t>
@@ -574,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AA54"/>
+  <dimension ref="B3:Y54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,29 +595,29 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -634,10 +628,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -655,10 +649,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
         <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -676,15 +670,15 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -692,23 +686,23 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -721,15 +715,15 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -737,18 +731,18 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>0</v>
       </c>
@@ -803,109 +797,97 @@
       <c r="S38" t="s">
         <v>31</v>
       </c>
-      <c r="T38" t="s">
-        <v>32</v>
-      </c>
-      <c r="U38" t="s">
-        <v>33</v>
+      <c r="T38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Y38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Z38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA38" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S39" t="s">
-        <v>43</v>
-      </c>
-      <c r="T39" t="s">
-        <v>43</v>
-      </c>
-      <c r="U39" t="s">
-        <v>43</v>
-      </c>
-      <c r="V39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W39" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-    </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>4</v>
       </c>
@@ -916,47 +898,47 @@
         <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F46" t="s">
         <v>2</v>
       </c>
       <c r="G46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" t="s">
+        <v>33</v>
+      </c>
+      <c r="I46" t="s">
         <v>34</v>
       </c>
-      <c r="H46" t="s">
+      <c r="J46" t="s">
         <v>35</v>
       </c>
-      <c r="I46" t="s">
-        <v>36</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>37</v>
       </c>
-      <c r="K46" t="s">
-        <v>39</v>
-      </c>
       <c r="L46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.25">
@@ -964,7 +946,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -973,16 +955,16 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H51" t="s">
         <v>46</v>
       </c>
-      <c r="G51" t="s">
+      <c r="I51" t="s">
         <v>47</v>
-      </c>
-      <c r="H51" t="s">
-        <v>48</v>
-      </c>
-      <c r="I51" t="s">
-        <v>49</v>
       </c>
       <c r="J51" t="s">
         <v>13</v>
@@ -991,27 +973,27 @@
         <v>2</v>
       </c>
       <c r="L51" t="s">
+        <v>32</v>
+      </c>
+      <c r="M51" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" t="s">
         <v>34</v>
       </c>
-      <c r="M51" t="s">
+      <c r="O51" t="s">
         <v>35</v>
       </c>
-      <c r="N51" t="s">
+      <c r="P51" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q51" t="s">
         <v>36</v>
-      </c>
-      <c r="O51" t="s">
-        <v>37</v>
-      </c>
-      <c r="P51" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.25">
@@ -1022,28 +1004,28 @@
         <v>10</v>
       </c>
       <c r="D54" t="s">
+        <v>55</v>
+      </c>
+      <c r="E54" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" t="s">
         <v>57</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>58</v>
       </c>
-      <c r="F54" t="s">
+      <c r="H54" t="s">
         <v>59</v>
       </c>
-      <c r="G54" t="s">
+      <c r="I54" t="s">
         <v>60</v>
       </c>
-      <c r="H54" t="s">
-        <v>61</v>
-      </c>
-      <c r="I54" t="s">
-        <v>62</v>
-      </c>
       <c r="J54" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update backend (add new models and migrations)
</commit_message>
<xml_diff>
--- a/ttf-backend/src/main/resources/db/scheme.xls.xlsx
+++ b/ttf-backend/src/main/resources/db/scheme.xls.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="98">
   <si>
     <t>Id</t>
   </si>
@@ -243,14 +244,98 @@
   </si>
   <si>
     <t>expiry_date</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>var(50)</t>
+  </si>
+  <si>
+    <t>var(120)</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>var(20)</t>
+  </si>
+  <si>
+    <t>teams</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>leagues</t>
+  </si>
+  <si>
+    <t>league_id</t>
+  </si>
+  <si>
+    <t>games_won</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>global_info</t>
+  </si>
+  <si>
+    <t>nbr_leagues</t>
+  </si>
+  <si>
+    <t>player1_id</t>
+  </si>
+  <si>
+    <t>player2_id</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>nbr_teams</t>
+  </si>
+  <si>
+    <t>season_info</t>
+  </si>
+  <si>
+    <t>end_status</t>
+  </si>
+  <si>
+    <t>score_lost</t>
+  </si>
+  <si>
+    <t>set_lost</t>
+  </si>
+  <si>
+    <t>games_lost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -273,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -281,13 +366,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W38" sqref="W38"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,4 +1185,783 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:Y49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="G5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="J5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="P10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="P13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="P15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="P16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="J19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U21" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="J29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="L31" t="s">
+        <v>50</v>
+      </c>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" t="s">
+        <v>26</v>
+      </c>
+      <c r="O36" t="s">
+        <v>27</v>
+      </c>
+      <c r="R36" t="s">
+        <v>30</v>
+      </c>
+      <c r="S36" t="s">
+        <v>31</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" t="s">
+        <v>41</v>
+      </c>
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" t="s">
+        <v>41</v>
+      </c>
+      <c r="J37" t="s">
+        <v>41</v>
+      </c>
+      <c r="K37" t="s">
+        <v>41</v>
+      </c>
+      <c r="L37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M37" t="s">
+        <v>41</v>
+      </c>
+      <c r="N37" t="s">
+        <v>41</v>
+      </c>
+      <c r="O37" t="s">
+        <v>41</v>
+      </c>
+      <c r="P37" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>29</v>
+      </c>
+      <c r="R37" t="s">
+        <v>41</v>
+      </c>
+      <c r="S37" t="s">
+        <v>41</v>
+      </c>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="L42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" t="s">
+        <v>46</v>
+      </c>
+      <c r="I46" t="s">
+        <v>47</v>
+      </c>
+      <c r="J46" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" t="s">
+        <v>2</v>
+      </c>
+      <c r="L46" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" t="s">
+        <v>33</v>
+      </c>
+      <c r="N46" t="s">
+        <v>34</v>
+      </c>
+      <c r="O46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49" t="s">
+        <v>58</v>
+      </c>
+      <c r="H49" t="s">
+        <v>59</v>
+      </c>
+      <c r="I49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update backend (all models and repositories)
</commit_message>
<xml_diff>
--- a/ttf-backend/src/main/resources/db/scheme.xls.xlsx
+++ b/ttf-backend/src/main/resources/db/scheme.xls.xlsx
@@ -1192,7 +1192,7 @@
   <dimension ref="B4:Y49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="K16" s="3"/>
       <c r="P16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q16" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
update backend (AddPlayer api)
</commit_message>
<xml_diff>
--- a/ttf-backend/src/main/resources/db/scheme.xls.xlsx
+++ b/ttf-backend/src/main/resources/db/scheme.xls.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="103">
   <si>
     <t>Id</t>
   </si>
@@ -319,6 +320,21 @@
   </si>
   <si>
     <t>games_lost</t>
+  </si>
+  <si>
+    <t>players</t>
+  </si>
+  <si>
+    <t>player_id</t>
+  </si>
+  <si>
+    <t>win_score</t>
+  </si>
+  <si>
+    <t>win_score3</t>
+  </si>
+  <si>
+    <t>lost_score2</t>
   </si>
 </sst>
 </file>
@@ -457,6 +473,2218 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>502103</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455009</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169307</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3550103" y="371475"/>
+          <a:ext cx="1781706" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>addNewMember</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>173756</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169307</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175531</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>72118</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4440956" y="740807"/>
+          <a:ext cx="1775" cy="283811"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>393245</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>93890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>491216</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3441245" y="1046390"/>
+          <a:ext cx="1926771" cy="696686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Send(user_id) form frnt</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>34015</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>88447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>262616</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99332</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Diamond 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3691615" y="1993447"/>
+          <a:ext cx="1447801" cy="1153885"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Players exists</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>137431</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>148316</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>88447</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4404631" y="1743076"/>
+          <a:ext cx="10885" cy="250371"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>44903</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>93890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>34015</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>93890</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3092903" y="2570390"/>
+          <a:ext cx="598712" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>240845</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>93890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>59567</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>82222</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3288845" y="2189390"/>
+          <a:ext cx="428322" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>no</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>23132</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55789</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>170089</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1666875" y="2309132"/>
+          <a:ext cx="1436914" cy="718457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Create new player</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>148316</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50347</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4410074" y="3147332"/>
+          <a:ext cx="5442" cy="522515"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>404131</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>110218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285756</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4671331" y="3158218"/>
+          <a:ext cx="491225" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419098</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>77560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>462641</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>131989</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Diamond 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3467098" y="3697060"/>
+          <a:ext cx="1872343" cy="1197429"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="800"/>
+            <a:t>Есть ли игрок в текущем сезоне если сезон =1, если сезон </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="800"/>
+            <a:t>&gt;1 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="800"/>
+            <a:t>то в сезоне +</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>131989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>136070</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4400550" y="4894489"/>
+          <a:ext cx="2720" cy="363311"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317045</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>415016</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3365045" y="5265965"/>
+          <a:ext cx="1926771" cy="696686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ru-RU"/>
+            <a:t>создаем профиль со статусом</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0"/>
+            <a:t>future</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556532</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>170088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317045</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Elbow Connector 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="16" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1581829" y="3831091"/>
+          <a:ext cx="2586719" cy="979713"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>193220</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>131990</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11942</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>120322</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4460420" y="4894490"/>
+          <a:ext cx="428322" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>no</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>462640</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93890</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5339440" y="4267200"/>
+          <a:ext cx="766085" cy="17690"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>604156</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485781</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>165225</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5480956" y="3796393"/>
+          <a:ext cx="491225" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12245</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>112940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>110216</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6108245" y="3922940"/>
+          <a:ext cx="1926771" cy="696686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ru-RU"/>
+            <a:t>заявка уже подана</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>43540</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>65315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4310740" y="5970815"/>
+          <a:ext cx="13610" cy="449035"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>278945</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>93890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>376916</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3326945" y="6380390"/>
+          <a:ext cx="1926771" cy="696686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ru-RU"/>
+            <a:t>заявка подана</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1189,10 +3417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Y49"/>
+  <dimension ref="B4:Y53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,11 +3428,12 @@
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
@@ -1218,7 +3447,7 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1238,7 +3467,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>74</v>
       </c>
@@ -1258,7 +3487,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>75</v>
       </c>
@@ -1272,7 +3501,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
@@ -1286,682 +3515,761 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F10" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="P10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T12" s="2" t="s">
+      <c r="P12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="U12" s="3"/>
-    </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="P13" s="4" t="s">
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Q13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T13" s="4" t="s">
+      <c r="P13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="U13" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P14" s="4" t="s">
+      <c r="T13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Q14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T14" s="4" t="s">
+      <c r="P14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U14" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="P15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T15" s="4" t="s">
+      <c r="P15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="U15" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="T15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="P16" s="4" t="s">
+      <c r="J16" s="3"/>
+      <c r="O16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T16" s="4" t="s">
+      <c r="P16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="U16" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T16" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T17" s="4" t="s">
+      <c r="P17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S17" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="U17" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" s="4" t="s">
+      <c r="T17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T18" s="4" t="s">
+      <c r="P18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="U18" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="T18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F19" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="J19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P19" s="4" t="s">
+      <c r="I19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T19" s="4" t="s">
+      <c r="P19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="U19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="T19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P20" s="4" t="s">
+      <c r="I20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F21" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="I21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="T21" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="I23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P21" s="4" t="s">
+      <c r="C27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K29" t="s">
+        <v>50</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>25</v>
+      </c>
+      <c r="N37" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J22" s="4" t="s">
+      <c r="O37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>41</v>
+      </c>
+      <c r="N38" t="s">
+        <v>41</v>
+      </c>
+      <c r="O38" t="s">
+        <v>41</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T22" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="U22" s="7" t="s">
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" t="s">
+        <v>30</v>
+      </c>
+      <c r="S39" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q23" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q25" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J26" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q26" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J28" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P28" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q28" s="5" t="s">
+      <c r="U39" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="6:21" x14ac:dyDescent="0.25">
-      <c r="J29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q29" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P30" s="6" t="s">
+      <c r="V39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y39" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="Q30" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="6:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J31" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="L31" t="s">
-        <v>50</v>
-      </c>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-    </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" t="s">
-        <v>22</v>
-      </c>
-      <c r="K36" t="s">
-        <v>23</v>
-      </c>
-      <c r="L36" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" t="s">
-        <v>25</v>
-      </c>
-      <c r="N36" t="s">
-        <v>26</v>
-      </c>
-      <c r="O36" t="s">
-        <v>27</v>
-      </c>
-      <c r="R36" t="s">
-        <v>30</v>
-      </c>
-      <c r="S36" t="s">
-        <v>31</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="X36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y36" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37" t="s">
-        <v>41</v>
-      </c>
-      <c r="H37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I37" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37" t="s">
-        <v>41</v>
-      </c>
-      <c r="L37" t="s">
-        <v>41</v>
-      </c>
-      <c r="M37" t="s">
-        <v>41</v>
-      </c>
-      <c r="N37" t="s">
-        <v>41</v>
-      </c>
-      <c r="O37" t="s">
-        <v>41</v>
-      </c>
-      <c r="P37" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>29</v>
-      </c>
-      <c r="R37" t="s">
-        <v>41</v>
-      </c>
-      <c r="S37" t="s">
-        <v>41</v>
-      </c>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-    </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="P38" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" t="s">
+        <v>41</v>
+      </c>
+      <c r="J40" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40" t="s">
+        <v>41</v>
+      </c>
+      <c r="L40" t="s">
+        <v>41</v>
+      </c>
+      <c r="P40" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>29</v>
+      </c>
+      <c r="R40" t="s">
+        <v>41</v>
+      </c>
+      <c r="S40" t="s">
+        <v>41</v>
+      </c>
+      <c r="V40" s="1"/>
+      <c r="Y40" s="1"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="P41" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
         <v>13</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D44" t="s">
         <v>16</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E44" t="s">
         <v>47</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F44" t="s">
         <v>2</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G44" t="s">
         <v>32</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H44" t="s">
         <v>33</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I44" t="s">
         <v>34</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J44" t="s">
         <v>35</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K44" t="s">
         <v>37</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L44" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" t="s">
-        <v>41</v>
-      </c>
-      <c r="L42" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>43</v>
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="L45" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>33</v>
+      </c>
+      <c r="N47" t="s">
+        <v>34</v>
+      </c>
+      <c r="O47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" t="s">
+        <v>47</v>
+      </c>
+      <c r="J49" t="s">
+        <v>13</v>
+      </c>
+      <c r="K49" t="s">
+        <v>2</v>
+      </c>
+      <c r="L49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>4</v>
       </c>
-      <c r="C46" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>44</v>
-      </c>
-      <c r="G46" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" t="s">
-        <v>46</v>
-      </c>
-      <c r="I46" t="s">
-        <v>47</v>
-      </c>
-      <c r="J46" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" t="s">
-        <v>2</v>
-      </c>
-      <c r="L46" t="s">
-        <v>32</v>
-      </c>
-      <c r="M46" t="s">
-        <v>33</v>
-      </c>
-      <c r="N46" t="s">
-        <v>34</v>
-      </c>
-      <c r="O46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="P47" t="s">
+      <c r="P50" t="s">
         <v>37</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="Q50" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" t="s">
+        <v>57</v>
+      </c>
+      <c r="G52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H52" t="s">
+        <v>59</v>
+      </c>
+      <c r="I52" t="s">
+        <v>60</v>
+      </c>
+      <c r="J52" t="s">
+        <v>52</v>
+      </c>
+      <c r="K52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>4</v>
-      </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" t="s">
-        <v>56</v>
-      </c>
-      <c r="F49" t="s">
-        <v>57</v>
-      </c>
-      <c r="G49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H49" t="s">
-        <v>59</v>
-      </c>
-      <c r="I49" t="s">
-        <v>60</v>
-      </c>
-      <c r="J49" t="s">
-        <v>52</v>
-      </c>
-      <c r="K49" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>